<commit_message>
Moved Add Record functionality to Track screen
</commit_message>
<xml_diff>
--- a/materials/dpsMappings.xlsx
+++ b/materials/dpsMappings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yuri\Desktop\Asakuki\materials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE14694E-F049-4E44-BAEF-10ABF1864801}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DD0584B-94D4-45BD-B6D1-AD6DD0DBC626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43080" yWindow="4680" windowWidth="28800" windowHeight="15345" xr2:uid="{501E6790-1055-43B6-8BFD-FEC52BB1AA7E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{501E6790-1055-43B6-8BFD-FEC52BB1AA7E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
   <si>
     <t>dps</t>
   </si>
@@ -111,6 +111,12 @@
   </si>
   <si>
     <t>Colour</t>
+  </si>
+  <si>
+    <t>0, 1</t>
+  </si>
+  <si>
+    <t>isEmpty</t>
   </si>
 </sst>
 </file>
@@ -159,15 +165,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -509,7 +512,7 @@
   <dimension ref="C3:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -559,25 +562,27 @@
       </c>
     </row>
     <row r="6" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C6" s="2">
+      <c r="C6" s="3">
         <v>12</v>
       </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="3">
-        <v>0</v>
+      <c r="D6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="H6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C7" s="4">
+      <c r="C7" s="3">
         <v>13</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="4" t="s">
         <v>20</v>
       </c>
       <c r="H7" t="s">
@@ -585,13 +590,13 @@
       </c>
     </row>
     <row r="8" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C8" s="4">
+      <c r="C8" s="3">
         <v>14</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="4" t="s">
         <v>19</v>
       </c>
       <c r="H8" t="s">

</xml_diff>